<commit_message>
Added Scenarios for Business Host - Single & Multiple
</commit_message>
<xml_diff>
--- a/CoOpsEvent/src/test/resources/TestData/Event_UI_QA_TestData.xlsx
+++ b/CoOpsEvent/src/test/resources/TestData/Event_UI_QA_TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aidenind-my.sharepoint.com/personal/monika_srivastava_aidenai_com/Documents/Documents/AidenAI/Event_Workspace/CoOpsEvent/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_DA7F552EF6E682C06DD4F76E21596CF690511DA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B04FD8-6D22-4E59-89A9-B2460EDABEB1}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="11_DA7F552EF6E682C06DD4F76E21596CF690511DA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{033BC124-D2F9-46A8-8598-CCFAD2178BAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>TestName</t>
   </si>
@@ -152,21 +152,9 @@
     <t>An account is already registered with this email address. Please enter a different email or log in.</t>
   </si>
   <si>
-    <t>monika.srivastava+mssingleindividual1testplayjavaauto1@aidenai.com</t>
-  </si>
-  <si>
-    <t>Monika Test Payment</t>
-  </si>
-  <si>
-    <t>monika.srivastava+msmultipleindividual1testplayjavaauto1@aidenai.com</t>
-  </si>
-  <si>
     <t>Event_Multiple_UI_Individual</t>
   </si>
   <si>
-    <t>Monika QA Payment</t>
-  </si>
-  <si>
     <t>Auction</t>
   </si>
   <si>
@@ -198,6 +186,66 @@
   </si>
   <si>
     <t>Coverage Days</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_SingleEvent_Business</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_MultipleEvents_Business</t>
+  </si>
+  <si>
+    <t>Bridal Shower</t>
+  </si>
+  <si>
+    <t>Event_Single_UI_Business</t>
+  </si>
+  <si>
+    <t>Event_Multiple_UI_Business</t>
+  </si>
+  <si>
+    <t>monika.srivastava+mssingleindividualauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>monika.srivastava+msmultipleindividualauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>monika.srivastava+mssinglebusinessauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>monika.srivastava+msmultiplebusinessauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>Monika Single Individual</t>
+  </si>
+  <si>
+    <t>Monika Multiple Individual</t>
+  </si>
+  <si>
+    <t>Monika Single Business</t>
+  </si>
+  <si>
+    <t>Monika Multiple Business</t>
+  </si>
+  <si>
+    <t>:40</t>
+  </si>
+  <si>
+    <t>06-30-2024</t>
+  </si>
+  <si>
+    <t>string:between 26-125</t>
+  </si>
+  <si>
+    <t>string:between 501-1,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auction </t>
+  </si>
+  <si>
+    <t>A Business</t>
+  </si>
+  <si>
+    <t>05-25-2024</t>
   </si>
 </sst>
 </file>
@@ -297,6 +345,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FDC3F5-6A9E-4B4A-B858-088A63CEF7DA}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,7 +660,7 @@
     <col min="16" max="19" width="36.88671875" customWidth="1"/>
     <col min="20" max="20" width="43.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
@@ -625,7 +677,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
@@ -690,13 +742,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2">
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2">
         <v>10</v>
@@ -708,7 +760,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K2" s="2">
         <v>8</v>
@@ -732,13 +784,13 @@
         <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="U2" s="2">
         <v>1557894561</v>
@@ -749,22 +801,22 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2">
         <v>8</v>
@@ -776,13 +828,13 @@
         <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2">
         <v>10</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>30</v>
@@ -794,25 +846,161 @@
         <v>25</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="U3" s="2">
         <v>1115557777</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="2">
+        <v>11</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1557773334</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="2">
+        <v>9</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1555999333</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -821,6 +1009,10 @@
     <hyperlink ref="T2" r:id="rId2" xr:uid="{15C710A4-3529-4C25-83A9-D53C7F37FAAB}"/>
     <hyperlink ref="O3" r:id="rId3" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{47BDD12F-48AB-420D-91E8-ECEC19EFEF49}"/>
     <hyperlink ref="T3" r:id="rId4" xr:uid="{CEE86AB6-41AE-4E01-934E-1FBAFE8525A8}"/>
+    <hyperlink ref="O4" r:id="rId5" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{EC2C0E19-55F9-4EE0-BF42-C2772C60C029}"/>
+    <hyperlink ref="T4" r:id="rId6" xr:uid="{2D247263-8484-4786-A874-86AF08C5F39E}"/>
+    <hyperlink ref="O5" r:id="rId7" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{DEB8DDD3-F0E4-4F0E-982E-981ADF3BE6CA}"/>
+    <hyperlink ref="T5" r:id="rId8" xr:uid="{A2D2C101-1F8E-4735-A1B7-F89370439BB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Event Scenarios -
</commit_message>
<xml_diff>
--- a/CoOpsEvent/src/test/resources/TestData/Event_UI_QA_TestData.xlsx
+++ b/CoOpsEvent/src/test/resources/TestData/Event_UI_QA_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aidenind-my.sharepoint.com/personal/monika_srivastava_aidenai_com/Documents/Documents/AidenAI/Event_Workspace/CoOpsEvent/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="11_DA7F552EF6E682C06DD4F76E21596CF690511DA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{033BC124-D2F9-46A8-8598-CCFAD2178BAD}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="11_DA7F552EF6E682C06DD4F76E21596CF690511DA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC0B5EEB-7E3C-47CD-931B-12A6F99FCEEF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,25 @@
     <sheet name="Event_E2E" sheetId="6" r:id="rId1"/>
     <sheet name="EventHosting" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="118">
   <si>
     <t>TestName</t>
   </si>
@@ -158,21 +171,9 @@
     <t>Auction</t>
   </si>
   <si>
-    <t>05-13-2024</t>
-  </si>
-  <si>
-    <t>05-20-2024</t>
-  </si>
-  <si>
-    <t>05-30-2024</t>
-  </si>
-  <si>
     <t>:15</t>
   </si>
   <si>
-    <t>05-17-2024</t>
-  </si>
-  <si>
     <t>validate_Event_E2EScenario_MultipleEvents_Individual</t>
   </si>
   <si>
@@ -227,9 +228,6 @@
     <t>Monika Multiple Business</t>
   </si>
   <si>
-    <t>:40</t>
-  </si>
-  <si>
     <t>06-30-2024</t>
   </si>
   <si>
@@ -245,7 +243,151 @@
     <t>A Business</t>
   </si>
   <si>
-    <t>05-25-2024</t>
+    <t>validate_Event_E2EScenario_SingleEvent_IndividualCoHost</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_MultipleEvents_IndividualInsureds</t>
+  </si>
+  <si>
+    <t>Baby Shower</t>
+  </si>
+  <si>
+    <t>303 Allstate Parkway, Markham, ON, Canada</t>
+  </si>
+  <si>
+    <t>:45</t>
+  </si>
+  <si>
+    <t>string:between 351-500</t>
+  </si>
+  <si>
+    <t>string:between 176-250</t>
+  </si>
+  <si>
+    <t>string:between 251-350</t>
+  </si>
+  <si>
+    <t>string:between 126-175</t>
+  </si>
+  <si>
+    <t>Monika Single Individual CoHost</t>
+  </si>
+  <si>
+    <t>Monika Multiple Individual Insureds</t>
+  </si>
+  <si>
+    <t>monika.srivastava+msmultipleindividualinsuredsauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>monika.srivastava+mssingleindividualcohostauto1@aidenai.com</t>
+  </si>
+  <si>
+    <t>Event_Single_UI_IndividualCoHost</t>
+  </si>
+  <si>
+    <t>Event_Multiple_UI_IndividualInsureds</t>
+  </si>
+  <si>
+    <t>Add Policy</t>
+  </si>
+  <si>
+    <t>Additional Insureds</t>
+  </si>
+  <si>
+    <t>Co-host</t>
+  </si>
+  <si>
+    <t>06-20-2024</t>
+  </si>
+  <si>
+    <t>06-25-2024</t>
+  </si>
+  <si>
+    <t>07-17-2024</t>
+  </si>
+  <si>
+    <t>07-13-2024</t>
+  </si>
+  <si>
+    <t>CoHost Name</t>
+  </si>
+  <si>
+    <t>CoHost Email</t>
+  </si>
+  <si>
+    <t>CoHost Single Business</t>
+  </si>
+  <si>
+    <t>CoHost Multiple Business</t>
+  </si>
+  <si>
+    <t>CoHost Single Indvidual</t>
+  </si>
+  <si>
+    <t>CoHost Multiple Individual</t>
+  </si>
+  <si>
+    <t>Event_Single_UI_DuplicateEmailAddress</t>
+  </si>
+  <si>
+    <t>monika.srivastava+duplicateemailaddress@aidenai.com</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_SingleEvent_DuplicateEmailAddress</t>
+  </si>
+  <si>
+    <t>600 Dixon Road, Etobicoke, ON, Canada</t>
+  </si>
+  <si>
+    <t>AddCard</t>
+  </si>
+  <si>
+    <t>CoHost Multiple Add Card</t>
+  </si>
+  <si>
+    <t>monika.srivastava+msmultiindiauto1addcard@aidenai.com</t>
+  </si>
+  <si>
+    <t>Event_Payment_AddCard</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_Payment_AddCard</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_MultipleEvents_AlcoholServed</t>
+  </si>
+  <si>
+    <t>Badminton</t>
+  </si>
+  <si>
+    <t>06-13-2024</t>
+  </si>
+  <si>
+    <t>06-17-2024</t>
+  </si>
+  <si>
+    <t>Event_Multiple_UI_AlcoholServed</t>
+  </si>
+  <si>
+    <t>Event_Multiple_UI_Sports_AlcoholServed</t>
+  </si>
+  <si>
+    <t>CoHost Multiple AlcoholServed</t>
+  </si>
+  <si>
+    <t>Monika Single Individual Sports</t>
+  </si>
+  <si>
+    <t>CoHost Single Indvidual AlcoholServed</t>
+  </si>
+  <si>
+    <t>validate_Event_E2EScenario_SingleEvent_Sports_AlcoholServed</t>
+  </si>
+  <si>
+    <t>string:30 or less</t>
   </si>
 </sst>
 </file>
@@ -255,7 +397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +417,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -322,13 +470,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,32 +789,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FDC3F5-6A9E-4B4A-B858-088A63CEF7DA}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
     <col min="11" max="13" width="17.6640625" customWidth="1"/>
     <col min="14" max="14" width="31.109375" customWidth="1"/>
     <col min="15" max="15" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="36.88671875" customWidth="1"/>
-    <col min="20" max="20" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.109375" customWidth="1"/>
+    <col min="21" max="21" width="36.88671875" customWidth="1"/>
+    <col min="22" max="22" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.88671875" customWidth="1"/>
+    <col min="24" max="24" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +832,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
@@ -719,19 +874,31 @@
         <v>37</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -742,13 +909,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2">
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="G2" s="2">
         <v>10</v>
@@ -760,7 +927,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="K2" s="2">
         <v>8</v>
@@ -784,39 +951,51 @@
         <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="U2" s="2">
+      <c r="X2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y2" s="2">
         <v>1557894561</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="G3" s="2">
         <v>8</v>
@@ -828,19 +1007,19 @@
         <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="K3" s="2">
         <v>10</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>30</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>25</v>
@@ -852,51 +1031,63 @@
         <v>41</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="U3" s="2">
+      <c r="X3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" s="2">
         <v>1115557777</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="G4" s="2">
         <v>6</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="K4" s="2">
         <v>11</v>
@@ -908,51 +1099,63 @@
         <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="U4" s="2">
+      <c r="X4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="2">
         <v>1557773334</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>58</v>
+      <c r="Z4" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2">
         <v>7</v>
@@ -964,57 +1167,576 @@
         <v>30</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K5" s="2">
         <v>9</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="N5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="6" t="str">
+        <f t="shared" ref="T5:T7" si="0">S2</f>
+        <v>No</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1555999333</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="2">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="2">
+        <v>11</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1557894561</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="2">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" s="2" t="s">
+      <c r="M7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="U5" s="2">
-        <v>1555999333</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>59</v>
+      <c r="X7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1115557777</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="2">
+        <v>8</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1557894561</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>1115557777</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="2">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="2">
+        <v>10</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>1115557777</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="2">
+        <v>8</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>1557894561</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{FABF4D44-A775-400C-BEDE-26CF3221A239}"/>
-    <hyperlink ref="T2" r:id="rId2" xr:uid="{15C710A4-3529-4C25-83A9-D53C7F37FAAB}"/>
+    <hyperlink ref="X2" r:id="rId2" xr:uid="{15C710A4-3529-4C25-83A9-D53C7F37FAAB}"/>
     <hyperlink ref="O3" r:id="rId3" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{47BDD12F-48AB-420D-91E8-ECEC19EFEF49}"/>
-    <hyperlink ref="T3" r:id="rId4" xr:uid="{CEE86AB6-41AE-4E01-934E-1FBAFE8525A8}"/>
+    <hyperlink ref="X3" r:id="rId4" xr:uid="{CEE86AB6-41AE-4E01-934E-1FBAFE8525A8}"/>
     <hyperlink ref="O4" r:id="rId5" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{EC2C0E19-55F9-4EE0-BF42-C2772C60C029}"/>
-    <hyperlink ref="T4" r:id="rId6" xr:uid="{2D247263-8484-4786-A874-86AF08C5F39E}"/>
+    <hyperlink ref="X4" r:id="rId6" xr:uid="{2D247263-8484-4786-A874-86AF08C5F39E}"/>
     <hyperlink ref="O5" r:id="rId7" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{DEB8DDD3-F0E4-4F0E-982E-981ADF3BE6CA}"/>
-    <hyperlink ref="T5" r:id="rId8" xr:uid="{A2D2C101-1F8E-4735-A1B7-F89370439BB2}"/>
+    <hyperlink ref="X5" r:id="rId8" xr:uid="{A2D2C101-1F8E-4735-A1B7-F89370439BB2}"/>
+    <hyperlink ref="O6" r:id="rId9" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{25343176-231D-4064-8C63-5AC39DF82916}"/>
+    <hyperlink ref="X6" r:id="rId10" xr:uid="{2F9D3A43-618C-4E2C-8297-010E0331B04A}"/>
+    <hyperlink ref="O7" r:id="rId11" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{C2A9417D-68BA-4D3B-8832-9050B82DE4B7}"/>
+    <hyperlink ref="X7" r:id="rId12" xr:uid="{C8DA67ED-1625-4811-81A5-D93013B9BF53}"/>
+    <hyperlink ref="V2" r:id="rId13" xr:uid="{E95E6760-4198-4082-99AE-E69B94FFA9CB}"/>
+    <hyperlink ref="V3" r:id="rId14" xr:uid="{8366F283-8C65-4095-BD4B-15CDE968664D}"/>
+    <hyperlink ref="V4" r:id="rId15" xr:uid="{3F6E31C5-89A5-4DB7-9C6E-1A2E9AF32E08}"/>
+    <hyperlink ref="V5" r:id="rId16" xr:uid="{4F4989A4-9F9B-4AE0-A551-C96F9FFCEC57}"/>
+    <hyperlink ref="V6" r:id="rId17" xr:uid="{31F8BF56-4C41-46BB-B321-B6D32A21A262}"/>
+    <hyperlink ref="V7" r:id="rId18" xr:uid="{ACE3F138-1392-4ED8-9AB8-1F64C6D2A98F}"/>
+    <hyperlink ref="O8" r:id="rId19" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{0945FA0B-FC42-4B4A-BBE4-610616B0FF9F}"/>
+    <hyperlink ref="X8" r:id="rId20" xr:uid="{8285C703-A16B-4FE7-8A81-BAB7320E1DCA}"/>
+    <hyperlink ref="V8" r:id="rId21" xr:uid="{C5192D85-004B-4CCF-AC72-BBBF2C2D3A2D}"/>
+    <hyperlink ref="O9" r:id="rId22" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{17394F5F-9FEF-4098-B635-1F561F5B0ACD}"/>
+    <hyperlink ref="X9" r:id="rId23" xr:uid="{50E3DD9D-1250-4245-B613-84DA2F01813C}"/>
+    <hyperlink ref="V9" r:id="rId24" xr:uid="{FC6CA740-7DEF-4F72-A240-0E3203E4A095}"/>
+    <hyperlink ref="O10" r:id="rId25" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{372204B8-F45F-4FB9-B613-65D97AE2C55B}"/>
+    <hyperlink ref="X10" r:id="rId26" xr:uid="{53F6BE0A-7048-4817-9D1F-EF415DF89AE6}"/>
+    <hyperlink ref="V10" r:id="rId27" xr:uid="{6A1B92FF-AEED-4C82-ACEB-2CB130001600}"/>
+    <hyperlink ref="O11" r:id="rId28" display="monika.srivastava+eventsingleindividual@aidenai.com" xr:uid="{9F8D9F8E-CD8C-4E26-BC1F-505EF1AE6AF0}"/>
+    <hyperlink ref="X11" r:id="rId29" xr:uid="{6079ECCD-5F65-46F9-9938-1785834EF6CC}"/>
+    <hyperlink ref="V11" r:id="rId30" xr:uid="{795890B8-7F08-41C0-808A-6094010AD1F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -1022,16 +1744,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8C25C9-6D30-4703-BC25-81785C98D6A3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1086,7 +1806,9 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>

</xml_diff>